<commit_message>
Ran 01.R again because I was missing UNFO7 at AguaFria and at this point I might never have clean data lol
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/01b_edited-species8_location-dependent-final-fix.xlsx
+++ b/data/data-wrangling-intermediate/01b_edited-species8_location-dependent-final-fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="13_ncr:40009_{0BA8441D-1008-43DB-A010-9C50448DAA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A2B9B70-8F0C-41C5-A33F-E2FD05A5E8A3}"/>
+  <xr:revisionPtr revIDLastSave="219" documentId="13_ncr:40009_{0BA8441D-1008-43DB-A010-9C50448DAA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFE80E7D-CD63-4774-B964-6B4FEB52B542}"/>
   <bookViews>
     <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1348,12 +1348,6 @@
     <t>UNFO5</t>
   </si>
   <si>
-    <t>UNFO5.AguaFria</t>
-  </si>
-  <si>
-    <t>Unknown forb 5, AguaFria</t>
-  </si>
-  <si>
     <t>UNFO5.FlyingM</t>
   </si>
   <si>
@@ -2735,6 +2729,12 @@
   </si>
   <si>
     <t>LUSP.AguaFria</t>
+  </si>
+  <si>
+    <t>UNFO7.AguaFria</t>
+  </si>
+  <si>
+    <t>Unknown forb 7, AguaFria</t>
   </si>
 </sst>
 </file>
@@ -3674,8 +3674,8 @@
   <dimension ref="A1:H347"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A304" sqref="A304:XFD304"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3801,19 +3801,19 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D5" t="s">
+        <v>725</v>
+      </c>
+      <c r="E5" t="s">
+        <v>796</v>
+      </c>
+      <c r="F5" t="s">
         <v>726</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>727</v>
-      </c>
-      <c r="E5" t="s">
-        <v>798</v>
-      </c>
-      <c r="F5" t="s">
-        <v>728</v>
-      </c>
-      <c r="G5" t="s">
-        <v>729</v>
       </c>
       <c r="H5" t="s">
         <v>44</v>
@@ -3879,13 +3879,13 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
+        <v>797</v>
+      </c>
+      <c r="D8" t="s">
+        <v>798</v>
+      </c>
+      <c r="E8" t="s">
         <v>799</v>
-      </c>
-      <c r="D8" t="s">
-        <v>800</v>
-      </c>
-      <c r="E8" t="s">
-        <v>801</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -3905,13 +3905,13 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
+        <v>660</v>
+      </c>
+      <c r="D9" t="s">
+        <v>661</v>
+      </c>
+      <c r="E9" t="s">
         <v>662</v>
-      </c>
-      <c r="D9" t="s">
-        <v>663</v>
-      </c>
-      <c r="E9" t="s">
-        <v>664</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -3931,13 +3931,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
+        <v>663</v>
+      </c>
+      <c r="D10" t="s">
+        <v>664</v>
+      </c>
+      <c r="E10" t="s">
         <v>665</v>
-      </c>
-      <c r="D10" t="s">
-        <v>666</v>
-      </c>
-      <c r="E10" t="s">
-        <v>667</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
@@ -3957,13 +3957,13 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
+        <v>666</v>
+      </c>
+      <c r="D11" t="s">
+        <v>667</v>
+      </c>
+      <c r="E11" t="s">
         <v>668</v>
-      </c>
-      <c r="D11" t="s">
-        <v>669</v>
-      </c>
-      <c r="E11" t="s">
-        <v>670</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -3983,13 +3983,13 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
+        <v>669</v>
+      </c>
+      <c r="D12" t="s">
+        <v>670</v>
+      </c>
+      <c r="E12" t="s">
         <v>671</v>
-      </c>
-      <c r="D12" t="s">
-        <v>672</v>
-      </c>
-      <c r="E12" t="s">
-        <v>673</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
@@ -4009,13 +4009,13 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D13" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E13" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
@@ -4035,13 +4035,13 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
+        <v>677</v>
+      </c>
+      <c r="D14" t="s">
+        <v>678</v>
+      </c>
+      <c r="E14" t="s">
         <v>679</v>
-      </c>
-      <c r="D14" t="s">
-        <v>680</v>
-      </c>
-      <c r="E14" t="s">
-        <v>681</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>13</v>
@@ -4061,13 +4061,13 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
+        <v>689</v>
+      </c>
+      <c r="D15" t="s">
+        <v>690</v>
+      </c>
+      <c r="E15" t="s">
         <v>691</v>
-      </c>
-      <c r="D15" t="s">
-        <v>692</v>
-      </c>
-      <c r="E15" t="s">
-        <v>693</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
@@ -4087,13 +4087,13 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
+        <v>693</v>
+      </c>
+      <c r="D16" t="s">
+        <v>694</v>
+      </c>
+      <c r="E16" t="s">
         <v>695</v>
-      </c>
-      <c r="D16" t="s">
-        <v>696</v>
-      </c>
-      <c r="E16" t="s">
-        <v>697</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -4113,13 +4113,13 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
+        <v>696</v>
+      </c>
+      <c r="D17" t="s">
+        <v>697</v>
+      </c>
+      <c r="E17" t="s">
         <v>698</v>
-      </c>
-      <c r="D17" t="s">
-        <v>699</v>
-      </c>
-      <c r="E17" t="s">
-        <v>700</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
@@ -4139,13 +4139,13 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
+        <v>702</v>
+      </c>
+      <c r="D18" t="s">
+        <v>703</v>
+      </c>
+      <c r="E18" t="s">
         <v>704</v>
-      </c>
-      <c r="D18" t="s">
-        <v>705</v>
-      </c>
-      <c r="E18" t="s">
-        <v>706</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
@@ -4165,13 +4165,13 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D19" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E19" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -4249,7 +4249,7 @@
         <v>333</v>
       </c>
       <c r="E22" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="F22" t="s">
         <v>14</v>
@@ -4269,13 +4269,13 @@
         <v>59</v>
       </c>
       <c r="C23" t="s">
+        <v>800</v>
+      </c>
+      <c r="D23" t="s">
+        <v>801</v>
+      </c>
+      <c r="E23" t="s">
         <v>802</v>
-      </c>
-      <c r="D23" t="s">
-        <v>803</v>
-      </c>
-      <c r="E23" t="s">
-        <v>804</v>
       </c>
       <c r="F23" t="s">
         <v>14</v>
@@ -4295,13 +4295,13 @@
         <v>59</v>
       </c>
       <c r="C24" t="s">
+        <v>621</v>
+      </c>
+      <c r="D24" t="s">
+        <v>622</v>
+      </c>
+      <c r="E24" t="s">
         <v>623</v>
-      </c>
-      <c r="D24" t="s">
-        <v>624</v>
-      </c>
-      <c r="E24" t="s">
-        <v>625</v>
       </c>
       <c r="F24" t="s">
         <v>5</v>
@@ -4321,13 +4321,13 @@
         <v>59</v>
       </c>
       <c r="C25" t="s">
+        <v>650</v>
+      </c>
+      <c r="D25" t="s">
+        <v>651</v>
+      </c>
+      <c r="E25" t="s">
         <v>652</v>
-      </c>
-      <c r="D25" t="s">
-        <v>653</v>
-      </c>
-      <c r="E25" t="s">
-        <v>654</v>
       </c>
       <c r="F25" t="s">
         <v>5</v>
@@ -4347,13 +4347,13 @@
         <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D26" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E26" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F26" t="s">
         <v>5</v>
@@ -4373,13 +4373,13 @@
         <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D27" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="E27" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -4399,13 +4399,13 @@
         <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="D28" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E28" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F28" t="s">
         <v>5</v>
@@ -4425,13 +4425,13 @@
         <v>59</v>
       </c>
       <c r="C29" t="s">
+        <v>673</v>
+      </c>
+      <c r="D29" t="s">
         <v>675</v>
       </c>
-      <c r="D29" t="s">
-        <v>677</v>
-      </c>
       <c r="E29" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="F29" t="s">
         <v>14</v>
@@ -4451,13 +4451,13 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
+        <v>680</v>
+      </c>
+      <c r="D30" t="s">
+        <v>681</v>
+      </c>
+      <c r="E30" t="s">
         <v>682</v>
-      </c>
-      <c r="D30" t="s">
-        <v>683</v>
-      </c>
-      <c r="E30" t="s">
-        <v>684</v>
       </c>
       <c r="F30" t="s">
         <v>14</v>
@@ -4477,13 +4477,13 @@
         <v>59</v>
       </c>
       <c r="C31" t="s">
+        <v>683</v>
+      </c>
+      <c r="D31" t="s">
+        <v>684</v>
+      </c>
+      <c r="E31" t="s">
         <v>685</v>
-      </c>
-      <c r="D31" t="s">
-        <v>686</v>
-      </c>
-      <c r="E31" t="s">
-        <v>687</v>
       </c>
       <c r="F31" t="s">
         <v>14</v>
@@ -4503,13 +4503,13 @@
         <v>59</v>
       </c>
       <c r="C32" t="s">
+        <v>686</v>
+      </c>
+      <c r="D32" t="s">
+        <v>687</v>
+      </c>
+      <c r="E32" t="s">
         <v>688</v>
-      </c>
-      <c r="D32" t="s">
-        <v>689</v>
-      </c>
-      <c r="E32" t="s">
-        <v>690</v>
       </c>
       <c r="F32" t="s">
         <v>14</v>
@@ -4529,13 +4529,13 @@
         <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D33" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E33" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F33" t="s">
         <v>5</v>
@@ -4555,13 +4555,13 @@
         <v>59</v>
       </c>
       <c r="C34" t="s">
+        <v>699</v>
+      </c>
+      <c r="D34" t="s">
+        <v>700</v>
+      </c>
+      <c r="E34" t="s">
         <v>701</v>
-      </c>
-      <c r="D34" t="s">
-        <v>702</v>
-      </c>
-      <c r="E34" t="s">
-        <v>703</v>
       </c>
       <c r="F34" t="s">
         <v>14</v>
@@ -4581,13 +4581,13 @@
         <v>59</v>
       </c>
       <c r="C35" t="s">
+        <v>705</v>
+      </c>
+      <c r="D35" t="s">
         <v>707</v>
       </c>
-      <c r="D35" t="s">
-        <v>709</v>
-      </c>
       <c r="E35" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="F35" t="s">
         <v>14</v>
@@ -4607,13 +4607,13 @@
         <v>59</v>
       </c>
       <c r="C36" t="s">
+        <v>708</v>
+      </c>
+      <c r="D36" t="s">
+        <v>709</v>
+      </c>
+      <c r="E36" t="s">
         <v>710</v>
-      </c>
-      <c r="D36" t="s">
-        <v>711</v>
-      </c>
-      <c r="E36" t="s">
-        <v>712</v>
       </c>
       <c r="F36" t="s">
         <v>5</v>
@@ -4685,10 +4685,10 @@
         <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D39" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E39" t="s">
         <v>223</v>
@@ -4867,13 +4867,13 @@
         <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>441</v>
+        <v>452</v>
       </c>
       <c r="D46" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="E46" t="s">
-        <v>443</v>
+        <v>454</v>
       </c>
       <c r="F46" t="s">
         <v>14</v>
@@ -4893,13 +4893,13 @@
         <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="D47" t="s">
-        <v>455</v>
+        <v>903</v>
       </c>
       <c r="E47" t="s">
-        <v>456</v>
+        <v>904</v>
       </c>
       <c r="F47" t="s">
         <v>14</v>
@@ -4919,13 +4919,13 @@
         <v>87</v>
       </c>
       <c r="C48" t="s">
+        <v>472</v>
+      </c>
+      <c r="D48" t="s">
+        <v>473</v>
+      </c>
+      <c r="E48" t="s">
         <v>474</v>
-      </c>
-      <c r="D48" t="s">
-        <v>475</v>
-      </c>
-      <c r="E48" t="s">
-        <v>476</v>
       </c>
       <c r="F48" t="s">
         <v>14</v>
@@ -4945,13 +4945,13 @@
         <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D49" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="E49" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="F49" t="s">
         <v>5</v>
@@ -4971,13 +4971,13 @@
         <v>87</v>
       </c>
       <c r="C50" t="s">
+        <v>547</v>
+      </c>
+      <c r="D50" t="s">
+        <v>548</v>
+      </c>
+      <c r="E50" t="s">
         <v>549</v>
-      </c>
-      <c r="D50" t="s">
-        <v>550</v>
-      </c>
-      <c r="E50" t="s">
-        <v>551</v>
       </c>
       <c r="F50" t="s">
         <v>5</v>
@@ -4997,13 +4997,13 @@
         <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D51" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="E51" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="F51" t="s">
         <v>5</v>
@@ -5023,13 +5023,13 @@
         <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D52" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E52" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F52" t="s">
         <v>5</v>
@@ -5049,13 +5049,13 @@
         <v>87</v>
       </c>
       <c r="C53" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D53" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="E53" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="F53" t="s">
         <v>14</v>
@@ -5075,13 +5075,13 @@
         <v>87</v>
       </c>
       <c r="C54" t="s">
+        <v>581</v>
+      </c>
+      <c r="D54" t="s">
+        <v>582</v>
+      </c>
+      <c r="E54" t="s">
         <v>583</v>
-      </c>
-      <c r="D54" t="s">
-        <v>584</v>
-      </c>
-      <c r="E54" t="s">
-        <v>585</v>
       </c>
       <c r="F54" t="s">
         <v>14</v>
@@ -5237,7 +5237,7 @@
         <v>179</v>
       </c>
       <c r="E60" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F60" t="s">
         <v>5</v>
@@ -5367,7 +5367,7 @@
         <v>321</v>
       </c>
       <c r="E65" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F65" t="s">
         <v>5</v>
@@ -5439,13 +5439,13 @@
         <v>33</v>
       </c>
       <c r="C68" t="s">
+        <v>528</v>
+      </c>
+      <c r="D68" t="s">
+        <v>529</v>
+      </c>
+      <c r="E68" t="s">
         <v>530</v>
-      </c>
-      <c r="D68" t="s">
-        <v>531</v>
-      </c>
-      <c r="E68" t="s">
-        <v>532</v>
       </c>
       <c r="F68" t="s">
         <v>14</v>
@@ -5465,13 +5465,13 @@
         <v>33</v>
       </c>
       <c r="C69" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D69" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E69" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F69" t="s">
         <v>5</v>
@@ -5491,13 +5491,13 @@
         <v>33</v>
       </c>
       <c r="C70" t="s">
+        <v>653</v>
+      </c>
+      <c r="D70" t="s">
+        <v>654</v>
+      </c>
+      <c r="E70" t="s">
         <v>655</v>
-      </c>
-      <c r="D70" t="s">
-        <v>656</v>
-      </c>
-      <c r="E70" t="s">
-        <v>657</v>
       </c>
       <c r="F70" t="s">
         <v>14</v>
@@ -5601,7 +5601,7 @@
         <v>93</v>
       </c>
       <c r="E74" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="F74" t="s">
         <v>5</v>
@@ -5780,10 +5780,10 @@
         <v>347</v>
       </c>
       <c r="D81" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E81" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="F81" t="s">
         <v>14</v>
@@ -5855,13 +5855,13 @@
         <v>26</v>
       </c>
       <c r="C84" t="s">
+        <v>815</v>
+      </c>
+      <c r="D84" t="s">
+        <v>816</v>
+      </c>
+      <c r="E84" t="s">
         <v>817</v>
-      </c>
-      <c r="D84" t="s">
-        <v>818</v>
-      </c>
-      <c r="E84" t="s">
-        <v>819</v>
       </c>
       <c r="F84" t="s">
         <v>14</v>
@@ -5907,13 +5907,13 @@
         <v>26</v>
       </c>
       <c r="C86" t="s">
+        <v>818</v>
+      </c>
+      <c r="D86" t="s">
+        <v>819</v>
+      </c>
+      <c r="E86" t="s">
         <v>820</v>
-      </c>
-      <c r="D86" t="s">
-        <v>821</v>
-      </c>
-      <c r="E86" t="s">
-        <v>822</v>
       </c>
       <c r="F86" t="s">
         <v>14</v>
@@ -5962,10 +5962,10 @@
         <v>388</v>
       </c>
       <c r="D88" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E88" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F88" t="s">
         <v>14</v>
@@ -6037,13 +6037,13 @@
         <v>26</v>
       </c>
       <c r="C91" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D91" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="E91" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="F91" t="s">
         <v>14</v>
@@ -6063,13 +6063,13 @@
         <v>26</v>
       </c>
       <c r="C92" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D92" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E92" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F92" t="s">
         <v>14</v>
@@ -6089,13 +6089,13 @@
         <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D93" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="E93" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="F93" t="s">
         <v>5</v>
@@ -6115,13 +6115,13 @@
         <v>26</v>
       </c>
       <c r="C94" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D94" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E94" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F94" t="s">
         <v>14</v>
@@ -6141,13 +6141,13 @@
         <v>26</v>
       </c>
       <c r="C95" t="s">
+        <v>618</v>
+      </c>
+      <c r="D95" t="s">
+        <v>619</v>
+      </c>
+      <c r="E95" t="s">
         <v>620</v>
-      </c>
-      <c r="D95" t="s">
-        <v>621</v>
-      </c>
-      <c r="E95" t="s">
-        <v>622</v>
       </c>
       <c r="F95" t="s">
         <v>14</v>
@@ -6277,7 +6277,7 @@
         <v>94</v>
       </c>
       <c r="E100" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="F100" t="s">
         <v>5</v>
@@ -6456,10 +6456,10 @@
         <v>344</v>
       </c>
       <c r="D107" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E107" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="F107" t="s">
         <v>5</v>
@@ -6612,10 +6612,10 @@
         <v>441</v>
       </c>
       <c r="D113" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E113" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F113" t="s">
         <v>14</v>
@@ -6635,13 +6635,13 @@
         <v>30</v>
       </c>
       <c r="C114" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D114" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E114" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F114" t="s">
         <v>14</v>
@@ -6661,13 +6661,13 @@
         <v>30</v>
       </c>
       <c r="C115" t="s">
+        <v>465</v>
+      </c>
+      <c r="D115" t="s">
+        <v>466</v>
+      </c>
+      <c r="E115" t="s">
         <v>467</v>
-      </c>
-      <c r="D115" t="s">
-        <v>468</v>
-      </c>
-      <c r="E115" t="s">
-        <v>469</v>
       </c>
       <c r="F115" t="s">
         <v>14</v>
@@ -6687,13 +6687,13 @@
         <v>30</v>
       </c>
       <c r="C116" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D116" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E116" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F116" t="s">
         <v>14</v>
@@ -6713,13 +6713,13 @@
         <v>30</v>
       </c>
       <c r="C117" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D117" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E117" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F117" t="s">
         <v>14</v>
@@ -6739,13 +6739,13 @@
         <v>30</v>
       </c>
       <c r="C118" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D118" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E118" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F118" t="s">
         <v>14</v>
@@ -6771,7 +6771,7 @@
         <v>96</v>
       </c>
       <c r="E119" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="F119" t="s">
         <v>5</v>
@@ -6817,19 +6817,19 @@
         <v>95</v>
       </c>
       <c r="C121" t="s">
+        <v>724</v>
+      </c>
+      <c r="D121" t="s">
+        <v>738</v>
+      </c>
+      <c r="E121" t="s">
+        <v>739</v>
+      </c>
+      <c r="F121" t="s">
         <v>726</v>
       </c>
-      <c r="D121" t="s">
-        <v>740</v>
-      </c>
-      <c r="E121" t="s">
-        <v>741</v>
-      </c>
-      <c r="F121" t="s">
-        <v>728</v>
-      </c>
       <c r="G121" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="H121" t="s">
         <v>44</v>
@@ -6846,10 +6846,10 @@
         <v>299</v>
       </c>
       <c r="D122" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E122" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F122" t="s">
         <v>13</v>
@@ -6976,10 +6976,10 @@
         <v>441</v>
       </c>
       <c r="D127" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E127" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F127" t="s">
         <v>14</v>
@@ -6999,13 +6999,13 @@
         <v>95</v>
       </c>
       <c r="C128" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D128" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E128" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F128" t="s">
         <v>14</v>
@@ -7025,13 +7025,13 @@
         <v>95</v>
       </c>
       <c r="C129" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D129" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E129" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F129" t="s">
         <v>14</v>
@@ -7051,13 +7051,13 @@
         <v>95</v>
       </c>
       <c r="C130" t="s">
+        <v>566</v>
+      </c>
+      <c r="D130" t="s">
+        <v>567</v>
+      </c>
+      <c r="E130" t="s">
         <v>568</v>
-      </c>
-      <c r="D130" t="s">
-        <v>569</v>
-      </c>
-      <c r="E130" t="s">
-        <v>570</v>
       </c>
       <c r="F130" t="s">
         <v>14</v>
@@ -7077,13 +7077,13 @@
         <v>95</v>
       </c>
       <c r="C131" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D131" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="E131" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="F131" t="s">
         <v>14</v>
@@ -7103,13 +7103,13 @@
         <v>95</v>
       </c>
       <c r="C132" t="s">
+        <v>576</v>
+      </c>
+      <c r="D132" t="s">
+        <v>577</v>
+      </c>
+      <c r="E132" t="s">
         <v>578</v>
-      </c>
-      <c r="D132" t="s">
-        <v>579</v>
-      </c>
-      <c r="E132" t="s">
-        <v>580</v>
       </c>
       <c r="F132" t="s">
         <v>14</v>
@@ -7161,7 +7161,7 @@
         <v>97</v>
       </c>
       <c r="E134" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="F134" t="s">
         <v>5</v>
@@ -7441,13 +7441,13 @@
         <v>70</v>
       </c>
       <c r="C145" t="s">
+        <v>829</v>
+      </c>
+      <c r="D145" t="s">
+        <v>830</v>
+      </c>
+      <c r="E145" t="s">
         <v>831</v>
-      </c>
-      <c r="D145" t="s">
-        <v>832</v>
-      </c>
-      <c r="E145" t="s">
-        <v>833</v>
       </c>
       <c r="F145" t="s">
         <v>14</v>
@@ -7467,13 +7467,13 @@
         <v>70</v>
       </c>
       <c r="C146" t="s">
+        <v>832</v>
+      </c>
+      <c r="D146" t="s">
+        <v>833</v>
+      </c>
+      <c r="E146" t="s">
         <v>834</v>
-      </c>
-      <c r="D146" t="s">
-        <v>835</v>
-      </c>
-      <c r="E146" t="s">
-        <v>836</v>
       </c>
       <c r="F146" t="s">
         <v>14</v>
@@ -7545,13 +7545,13 @@
         <v>70</v>
       </c>
       <c r="C149" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D149" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E149" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F149" t="s">
         <v>14</v>
@@ -7571,13 +7571,13 @@
         <v>70</v>
       </c>
       <c r="C150" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D150" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E150" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F150" t="s">
         <v>5</v>
@@ -7597,13 +7597,13 @@
         <v>70</v>
       </c>
       <c r="C151" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D151" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E151" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F151" t="s">
         <v>14</v>
@@ -7623,13 +7623,13 @@
         <v>70</v>
       </c>
       <c r="C152" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D152" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E152" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="F152" t="s">
         <v>5</v>
@@ -7649,13 +7649,13 @@
         <v>70</v>
       </c>
       <c r="C153" t="s">
+        <v>742</v>
+      </c>
+      <c r="D153" t="s">
+        <v>743</v>
+      </c>
+      <c r="E153" t="s">
         <v>744</v>
-      </c>
-      <c r="D153" t="s">
-        <v>745</v>
-      </c>
-      <c r="E153" t="s">
-        <v>746</v>
       </c>
       <c r="F153" t="s">
         <v>14</v>
@@ -7675,13 +7675,13 @@
         <v>70</v>
       </c>
       <c r="C154" t="s">
+        <v>657</v>
+      </c>
+      <c r="D154" t="s">
+        <v>658</v>
+      </c>
+      <c r="E154" t="s">
         <v>659</v>
-      </c>
-      <c r="D154" t="s">
-        <v>660</v>
-      </c>
-      <c r="E154" t="s">
-        <v>661</v>
       </c>
       <c r="F154" t="s">
         <v>14</v>
@@ -7733,7 +7733,7 @@
         <v>98</v>
       </c>
       <c r="E156" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="F156" t="s">
         <v>5</v>
@@ -7990,10 +7990,10 @@
         <v>441</v>
       </c>
       <c r="D166" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E166" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F166" t="s">
         <v>14</v>
@@ -8013,13 +8013,13 @@
         <v>22</v>
       </c>
       <c r="C167" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D167" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E167" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F167" t="s">
         <v>14</v>
@@ -8039,13 +8039,13 @@
         <v>22</v>
       </c>
       <c r="C168" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D168" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E168" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F168" t="s">
         <v>14</v>
@@ -8065,13 +8065,13 @@
         <v>22</v>
       </c>
       <c r="C169" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D169" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E169" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F169" t="s">
         <v>14</v>
@@ -8091,13 +8091,13 @@
         <v>22</v>
       </c>
       <c r="C170" t="s">
+        <v>481</v>
+      </c>
+      <c r="D170" t="s">
+        <v>482</v>
+      </c>
+      <c r="E170" t="s">
         <v>483</v>
-      </c>
-      <c r="D170" t="s">
-        <v>484</v>
-      </c>
-      <c r="E170" t="s">
-        <v>485</v>
       </c>
       <c r="F170" t="s">
         <v>14</v>
@@ -8117,13 +8117,13 @@
         <v>22</v>
       </c>
       <c r="C171" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D171" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E171" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F171" t="s">
         <v>14</v>
@@ -8143,13 +8143,13 @@
         <v>22</v>
       </c>
       <c r="C172" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D172" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E172" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F172" t="s">
         <v>14</v>
@@ -8169,13 +8169,13 @@
         <v>22</v>
       </c>
       <c r="C173" t="s">
+        <v>612</v>
+      </c>
+      <c r="D173" t="s">
+        <v>613</v>
+      </c>
+      <c r="E173" t="s">
         <v>614</v>
-      </c>
-      <c r="D173" t="s">
-        <v>615</v>
-      </c>
-      <c r="E173" t="s">
-        <v>616</v>
       </c>
       <c r="F173" t="s">
         <v>14</v>
@@ -8305,7 +8305,7 @@
         <v>328</v>
       </c>
       <c r="E178" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="F178" t="s">
         <v>5</v>
@@ -8377,13 +8377,13 @@
         <v>73</v>
       </c>
       <c r="C181" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D181" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E181" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F181" t="s">
         <v>14</v>
@@ -8715,13 +8715,13 @@
         <v>139</v>
       </c>
       <c r="C194" t="s">
+        <v>837</v>
+      </c>
+      <c r="D194" t="s">
+        <v>838</v>
+      </c>
+      <c r="E194" t="s">
         <v>839</v>
-      </c>
-      <c r="D194" t="s">
-        <v>840</v>
-      </c>
-      <c r="E194" t="s">
-        <v>841</v>
       </c>
       <c r="F194" t="s">
         <v>14</v>
@@ -8738,16 +8738,16 @@
         <v>140</v>
       </c>
       <c r="B195" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C195" t="s">
         <v>142</v>
       </c>
       <c r="D195" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E195" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="F195" t="s">
         <v>5</v>
@@ -8764,16 +8764,16 @@
         <v>140</v>
       </c>
       <c r="B196" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C196" t="s">
+        <v>748</v>
+      </c>
+      <c r="D196" t="s">
+        <v>749</v>
+      </c>
+      <c r="E196" t="s">
         <v>750</v>
-      </c>
-      <c r="D196" t="s">
-        <v>751</v>
-      </c>
-      <c r="E196" t="s">
-        <v>752</v>
       </c>
       <c r="F196" t="s">
         <v>5</v>
@@ -8790,16 +8790,16 @@
         <v>140</v>
       </c>
       <c r="B197" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C197" t="s">
+        <v>751</v>
+      </c>
+      <c r="D197" t="s">
+        <v>752</v>
+      </c>
+      <c r="E197" t="s">
         <v>753</v>
-      </c>
-      <c r="D197" t="s">
-        <v>754</v>
-      </c>
-      <c r="E197" t="s">
-        <v>755</v>
       </c>
       <c r="F197" t="s">
         <v>13</v>
@@ -8816,16 +8816,16 @@
         <v>140</v>
       </c>
       <c r="B198" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C198" t="s">
+        <v>754</v>
+      </c>
+      <c r="D198" t="s">
+        <v>755</v>
+      </c>
+      <c r="E198" t="s">
         <v>756</v>
-      </c>
-      <c r="D198" t="s">
-        <v>757</v>
-      </c>
-      <c r="E198" t="s">
-        <v>758</v>
       </c>
       <c r="F198" t="s">
         <v>5</v>
@@ -8842,16 +8842,16 @@
         <v>140</v>
       </c>
       <c r="B199" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C199" t="s">
+        <v>757</v>
+      </c>
+      <c r="D199" t="s">
+        <v>758</v>
+      </c>
+      <c r="E199" t="s">
         <v>759</v>
-      </c>
-      <c r="D199" t="s">
-        <v>760</v>
-      </c>
-      <c r="E199" t="s">
-        <v>761</v>
       </c>
       <c r="F199" t="s">
         <v>14</v>
@@ -8868,16 +8868,16 @@
         <v>140</v>
       </c>
       <c r="B200" t="s">
+        <v>624</v>
+      </c>
+      <c r="C200" t="s">
+        <v>625</v>
+      </c>
+      <c r="D200" t="s">
         <v>626</v>
       </c>
-      <c r="C200" t="s">
+      <c r="E200" t="s">
         <v>627</v>
-      </c>
-      <c r="D200" t="s">
-        <v>628</v>
-      </c>
-      <c r="E200" t="s">
-        <v>629</v>
       </c>
       <c r="F200" t="s">
         <v>14</v>
@@ -8894,16 +8894,16 @@
         <v>140</v>
       </c>
       <c r="B201" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C201" t="s">
+        <v>631</v>
+      </c>
+      <c r="D201" t="s">
+        <v>632</v>
+      </c>
+      <c r="E201" t="s">
         <v>633</v>
-      </c>
-      <c r="D201" t="s">
-        <v>634</v>
-      </c>
-      <c r="E201" t="s">
-        <v>635</v>
       </c>
       <c r="F201" t="s">
         <v>14</v>
@@ -8920,16 +8920,16 @@
         <v>140</v>
       </c>
       <c r="B202" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C202" t="s">
+        <v>637</v>
+      </c>
+      <c r="D202" t="s">
+        <v>638</v>
+      </c>
+      <c r="E202" t="s">
         <v>639</v>
-      </c>
-      <c r="D202" t="s">
-        <v>640</v>
-      </c>
-      <c r="E202" t="s">
-        <v>641</v>
       </c>
       <c r="F202" t="s">
         <v>14</v>
@@ -8946,16 +8946,16 @@
         <v>140</v>
       </c>
       <c r="B203" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C203" t="s">
+        <v>645</v>
+      </c>
+      <c r="D203" t="s">
+        <v>646</v>
+      </c>
+      <c r="E203" t="s">
         <v>647</v>
-      </c>
-      <c r="D203" t="s">
-        <v>648</v>
-      </c>
-      <c r="E203" t="s">
-        <v>649</v>
       </c>
       <c r="F203" t="s">
         <v>14</v>
@@ -9001,19 +9001,19 @@
         <v>141</v>
       </c>
       <c r="C205" t="s">
+        <v>724</v>
+      </c>
+      <c r="D205" t="s">
+        <v>760</v>
+      </c>
+      <c r="E205" t="s">
+        <v>761</v>
+      </c>
+      <c r="F205" t="s">
         <v>726</v>
       </c>
-      <c r="D205" t="s">
-        <v>762</v>
-      </c>
-      <c r="E205" t="s">
-        <v>763</v>
-      </c>
-      <c r="F205" t="s">
-        <v>728</v>
-      </c>
       <c r="G205" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="H205" t="s">
         <v>44</v>
@@ -9027,13 +9027,13 @@
         <v>141</v>
       </c>
       <c r="C206" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D206" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E206" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="F206" t="s">
         <v>14</v>
@@ -9053,13 +9053,13 @@
         <v>141</v>
       </c>
       <c r="C207" t="s">
+        <v>628</v>
+      </c>
+      <c r="D207" t="s">
+        <v>629</v>
+      </c>
+      <c r="E207" t="s">
         <v>630</v>
-      </c>
-      <c r="D207" t="s">
-        <v>631</v>
-      </c>
-      <c r="E207" t="s">
-        <v>632</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>13</v>
@@ -9079,13 +9079,13 @@
         <v>141</v>
       </c>
       <c r="C208" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D208" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="E208" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F208" t="s">
         <v>14</v>
@@ -9131,13 +9131,13 @@
         <v>145</v>
       </c>
       <c r="C210" t="s">
+        <v>634</v>
+      </c>
+      <c r="D210" t="s">
+        <v>635</v>
+      </c>
+      <c r="E210" t="s">
         <v>636</v>
-      </c>
-      <c r="D210" t="s">
-        <v>637</v>
-      </c>
-      <c r="E210" t="s">
-        <v>638</v>
       </c>
       <c r="F210" t="s">
         <v>14</v>
@@ -9157,13 +9157,13 @@
         <v>145</v>
       </c>
       <c r="C211" t="s">
+        <v>711</v>
+      </c>
+      <c r="D211" t="s">
+        <v>712</v>
+      </c>
+      <c r="E211" t="s">
         <v>713</v>
-      </c>
-      <c r="D211" t="s">
-        <v>714</v>
-      </c>
-      <c r="E211" t="s">
-        <v>715</v>
       </c>
       <c r="F211" t="s">
         <v>14</v>
@@ -9183,13 +9183,13 @@
         <v>145</v>
       </c>
       <c r="C212" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D212" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="E212" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F212" t="s">
         <v>14</v>
@@ -9209,13 +9209,13 @@
         <v>145</v>
       </c>
       <c r="C213" t="s">
+        <v>840</v>
+      </c>
+      <c r="D213" t="s">
+        <v>841</v>
+      </c>
+      <c r="E213" t="s">
         <v>842</v>
-      </c>
-      <c r="D213" t="s">
-        <v>843</v>
-      </c>
-      <c r="E213" t="s">
-        <v>844</v>
       </c>
       <c r="F213" t="s">
         <v>14</v>
@@ -9232,16 +9232,16 @@
         <v>140</v>
       </c>
       <c r="B214" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C214" t="s">
+        <v>843</v>
+      </c>
+      <c r="D214" t="s">
+        <v>844</v>
+      </c>
+      <c r="E214" t="s">
         <v>845</v>
-      </c>
-      <c r="D214" t="s">
-        <v>846</v>
-      </c>
-      <c r="E214" t="s">
-        <v>847</v>
       </c>
       <c r="F214" t="s">
         <v>14</v>
@@ -9258,16 +9258,16 @@
         <v>140</v>
       </c>
       <c r="B215" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C215" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D215" t="s">
+        <v>640</v>
+      </c>
+      <c r="E215" t="s">
         <v>642</v>
-      </c>
-      <c r="E215" t="s">
-        <v>644</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>5</v>
@@ -9284,16 +9284,16 @@
         <v>140</v>
       </c>
       <c r="B216" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C216" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D216" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E216" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F216" t="s">
         <v>14</v>
@@ -9310,16 +9310,16 @@
         <v>140</v>
       </c>
       <c r="B217" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C217" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D217" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="E217" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="F217" t="s">
         <v>14</v>
@@ -9452,7 +9452,7 @@
         <v>182</v>
       </c>
       <c r="F222" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G222" t="s">
         <v>14</v>
@@ -9475,7 +9475,7 @@
         <v>192</v>
       </c>
       <c r="E223" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F223" t="s">
         <v>5</v>
@@ -9547,13 +9547,13 @@
         <v>40</v>
       </c>
       <c r="C226" t="s">
+        <v>764</v>
+      </c>
+      <c r="D226" t="s">
+        <v>765</v>
+      </c>
+      <c r="E226" t="s">
         <v>766</v>
-      </c>
-      <c r="D226" t="s">
-        <v>767</v>
-      </c>
-      <c r="E226" t="s">
-        <v>768</v>
       </c>
       <c r="F226" t="s">
         <v>13</v>
@@ -9576,10 +9576,10 @@
         <v>290</v>
       </c>
       <c r="D227" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E227" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="F227" t="s">
         <v>13</v>
@@ -9599,13 +9599,13 @@
         <v>40</v>
       </c>
       <c r="C228" t="s">
+        <v>769</v>
+      </c>
+      <c r="D228" t="s">
+        <v>770</v>
+      </c>
+      <c r="E228" t="s">
         <v>771</v>
-      </c>
-      <c r="D228" t="s">
-        <v>772</v>
-      </c>
-      <c r="E228" t="s">
-        <v>773</v>
       </c>
       <c r="F228" t="s">
         <v>14</v>
@@ -9657,7 +9657,7 @@
         <v>387</v>
       </c>
       <c r="E230" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F230" t="s">
         <v>14</v>
@@ -9732,10 +9732,10 @@
         <v>441</v>
       </c>
       <c r="D233" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E233" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F233" t="s">
         <v>14</v>
@@ -9755,13 +9755,13 @@
         <v>40</v>
       </c>
       <c r="C234" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D234" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E234" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F234" t="s">
         <v>14</v>
@@ -9781,13 +9781,13 @@
         <v>40</v>
       </c>
       <c r="C235" t="s">
+        <v>486</v>
+      </c>
+      <c r="D235" t="s">
+        <v>487</v>
+      </c>
+      <c r="E235" t="s">
         <v>488</v>
-      </c>
-      <c r="D235" t="s">
-        <v>489</v>
-      </c>
-      <c r="E235" t="s">
-        <v>490</v>
       </c>
       <c r="F235" t="s">
         <v>14</v>
@@ -9807,13 +9807,13 @@
         <v>40</v>
       </c>
       <c r="C236" t="s">
+        <v>489</v>
+      </c>
+      <c r="D236" t="s">
+        <v>490</v>
+      </c>
+      <c r="E236" t="s">
         <v>491</v>
-      </c>
-      <c r="D236" t="s">
-        <v>492</v>
-      </c>
-      <c r="E236" t="s">
-        <v>493</v>
       </c>
       <c r="F236" t="s">
         <v>13</v>
@@ -9833,13 +9833,13 @@
         <v>40</v>
       </c>
       <c r="C237" t="s">
+        <v>492</v>
+      </c>
+      <c r="D237" t="s">
+        <v>493</v>
+      </c>
+      <c r="E237" t="s">
         <v>494</v>
-      </c>
-      <c r="D237" t="s">
-        <v>495</v>
-      </c>
-      <c r="E237" t="s">
-        <v>496</v>
       </c>
       <c r="F237" t="s">
         <v>14</v>
@@ -9859,13 +9859,13 @@
         <v>40</v>
       </c>
       <c r="C238" t="s">
+        <v>495</v>
+      </c>
+      <c r="D238" t="s">
+        <v>496</v>
+      </c>
+      <c r="E238" t="s">
         <v>497</v>
-      </c>
-      <c r="D238" t="s">
-        <v>498</v>
-      </c>
-      <c r="E238" t="s">
-        <v>499</v>
       </c>
       <c r="F238" t="s">
         <v>13</v>
@@ -9885,13 +9885,13 @@
         <v>40</v>
       </c>
       <c r="C239" t="s">
+        <v>498</v>
+      </c>
+      <c r="D239" t="s">
+        <v>499</v>
+      </c>
+      <c r="E239" t="s">
         <v>500</v>
-      </c>
-      <c r="D239" t="s">
-        <v>501</v>
-      </c>
-      <c r="E239" t="s">
-        <v>502</v>
       </c>
       <c r="F239" t="s">
         <v>13</v>
@@ -9911,13 +9911,13 @@
         <v>40</v>
       </c>
       <c r="C240" t="s">
+        <v>501</v>
+      </c>
+      <c r="D240" t="s">
+        <v>502</v>
+      </c>
+      <c r="E240" t="s">
         <v>503</v>
-      </c>
-      <c r="D240" t="s">
-        <v>504</v>
-      </c>
-      <c r="E240" t="s">
-        <v>505</v>
       </c>
       <c r="F240" t="s">
         <v>14</v>
@@ -9937,13 +9937,13 @@
         <v>40</v>
       </c>
       <c r="C241" t="s">
+        <v>504</v>
+      </c>
+      <c r="D241" t="s">
+        <v>505</v>
+      </c>
+      <c r="E241" t="s">
         <v>506</v>
-      </c>
-      <c r="D241" t="s">
-        <v>507</v>
-      </c>
-      <c r="E241" t="s">
-        <v>508</v>
       </c>
       <c r="F241" t="s">
         <v>14</v>
@@ -9963,13 +9963,13 @@
         <v>40</v>
       </c>
       <c r="C242" t="s">
+        <v>522</v>
+      </c>
+      <c r="D242" t="s">
+        <v>523</v>
+      </c>
+      <c r="E242" t="s">
         <v>524</v>
-      </c>
-      <c r="D242" t="s">
-        <v>525</v>
-      </c>
-      <c r="E242" t="s">
-        <v>526</v>
       </c>
       <c r="F242" t="s">
         <v>14</v>
@@ -9989,13 +9989,13 @@
         <v>40</v>
       </c>
       <c r="C243" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D243" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E243" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F243" t="s">
         <v>14</v>
@@ -10015,13 +10015,13 @@
         <v>40</v>
       </c>
       <c r="C244" t="s">
+        <v>586</v>
+      </c>
+      <c r="D244" t="s">
+        <v>587</v>
+      </c>
+      <c r="E244" t="s">
         <v>588</v>
-      </c>
-      <c r="D244" t="s">
-        <v>589</v>
-      </c>
-      <c r="E244" t="s">
-        <v>590</v>
       </c>
       <c r="F244" t="s">
         <v>13</v>
@@ -10041,13 +10041,13 @@
         <v>40</v>
       </c>
       <c r="C245" t="s">
+        <v>590</v>
+      </c>
+      <c r="D245" t="s">
+        <v>591</v>
+      </c>
+      <c r="E245" t="s">
         <v>592</v>
-      </c>
-      <c r="D245" t="s">
-        <v>593</v>
-      </c>
-      <c r="E245" t="s">
-        <v>594</v>
       </c>
       <c r="F245" t="s">
         <v>14</v>
@@ -10067,13 +10067,13 @@
         <v>40</v>
       </c>
       <c r="C246" t="s">
+        <v>593</v>
+      </c>
+      <c r="D246" t="s">
+        <v>594</v>
+      </c>
+      <c r="E246" t="s">
         <v>595</v>
-      </c>
-      <c r="D246" t="s">
-        <v>596</v>
-      </c>
-      <c r="E246" t="s">
-        <v>597</v>
       </c>
       <c r="F246" t="s">
         <v>5</v>
@@ -10093,13 +10093,13 @@
         <v>40</v>
       </c>
       <c r="C247" t="s">
+        <v>596</v>
+      </c>
+      <c r="D247" t="s">
+        <v>597</v>
+      </c>
+      <c r="E247" t="s">
         <v>598</v>
-      </c>
-      <c r="D247" t="s">
-        <v>599</v>
-      </c>
-      <c r="E247" t="s">
-        <v>600</v>
       </c>
       <c r="F247" t="s">
         <v>5</v>
@@ -10119,13 +10119,13 @@
         <v>40</v>
       </c>
       <c r="C248" t="s">
+        <v>773</v>
+      </c>
+      <c r="D248" t="s">
+        <v>774</v>
+      </c>
+      <c r="E248" t="s">
         <v>775</v>
-      </c>
-      <c r="D248" t="s">
-        <v>776</v>
-      </c>
-      <c r="E248" t="s">
-        <v>777</v>
       </c>
       <c r="F248" t="s">
         <v>5</v>
@@ -10405,10 +10405,10 @@
         <v>9</v>
       </c>
       <c r="C259" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D259" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E259" t="s">
         <v>101</v>
@@ -10431,10 +10431,10 @@
         <v>9</v>
       </c>
       <c r="C260" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D260" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E260" t="s">
         <v>101</v>
@@ -10561,7 +10561,7 @@
         <v>9</v>
       </c>
       <c r="C265" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D265" t="s">
         <v>106</v>
@@ -10613,13 +10613,13 @@
         <v>9</v>
       </c>
       <c r="C267" t="s">
+        <v>846</v>
+      </c>
+      <c r="D267" t="s">
+        <v>847</v>
+      </c>
+      <c r="E267" t="s">
         <v>848</v>
-      </c>
-      <c r="D267" t="s">
-        <v>849</v>
-      </c>
-      <c r="E267" t="s">
-        <v>850</v>
       </c>
       <c r="F267" t="s">
         <v>5</v>
@@ -10639,13 +10639,13 @@
         <v>9</v>
       </c>
       <c r="C268" t="s">
+        <v>849</v>
+      </c>
+      <c r="D268" t="s">
+        <v>850</v>
+      </c>
+      <c r="E268" t="s">
         <v>851</v>
-      </c>
-      <c r="D268" t="s">
-        <v>852</v>
-      </c>
-      <c r="E268" t="s">
-        <v>853</v>
       </c>
       <c r="F268" t="s">
         <v>5</v>
@@ -10691,13 +10691,13 @@
         <v>9</v>
       </c>
       <c r="C270" t="s">
+        <v>852</v>
+      </c>
+      <c r="D270" t="s">
+        <v>853</v>
+      </c>
+      <c r="E270" t="s">
         <v>854</v>
-      </c>
-      <c r="D270" t="s">
-        <v>855</v>
-      </c>
-      <c r="E270" t="s">
-        <v>856</v>
       </c>
       <c r="F270" t="s">
         <v>5</v>
@@ -10717,13 +10717,13 @@
         <v>9</v>
       </c>
       <c r="C271" t="s">
+        <v>855</v>
+      </c>
+      <c r="D271" t="s">
+        <v>856</v>
+      </c>
+      <c r="E271" t="s">
         <v>857</v>
-      </c>
-      <c r="D271" t="s">
-        <v>858</v>
-      </c>
-      <c r="E271" t="s">
-        <v>859</v>
       </c>
       <c r="F271" t="s">
         <v>5</v>
@@ -10743,13 +10743,13 @@
         <v>9</v>
       </c>
       <c r="C272" t="s">
+        <v>858</v>
+      </c>
+      <c r="D272" t="s">
+        <v>859</v>
+      </c>
+      <c r="E272" t="s">
         <v>860</v>
-      </c>
-      <c r="D272" t="s">
-        <v>861</v>
-      </c>
-      <c r="E272" t="s">
-        <v>862</v>
       </c>
       <c r="F272" t="s">
         <v>5</v>
@@ -10769,13 +10769,13 @@
         <v>9</v>
       </c>
       <c r="C273" t="s">
+        <v>861</v>
+      </c>
+      <c r="D273" t="s">
+        <v>862</v>
+      </c>
+      <c r="E273" t="s">
         <v>863</v>
-      </c>
-      <c r="D273" t="s">
-        <v>864</v>
-      </c>
-      <c r="E273" t="s">
-        <v>865</v>
       </c>
       <c r="F273" t="s">
         <v>5</v>
@@ -10795,13 +10795,13 @@
         <v>9</v>
       </c>
       <c r="C274" t="s">
+        <v>864</v>
+      </c>
+      <c r="D274" t="s">
+        <v>865</v>
+      </c>
+      <c r="E274" t="s">
         <v>866</v>
-      </c>
-      <c r="D274" t="s">
-        <v>867</v>
-      </c>
-      <c r="E274" t="s">
-        <v>868</v>
       </c>
       <c r="F274" t="s">
         <v>5</v>
@@ -10824,10 +10824,10 @@
         <v>199</v>
       </c>
       <c r="D275" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E275" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F275" t="s">
         <v>5</v>
@@ -11055,13 +11055,13 @@
         <v>9</v>
       </c>
       <c r="C284" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D284" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E284" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F284" t="s">
         <v>14</v>
@@ -11081,13 +11081,13 @@
         <v>9</v>
       </c>
       <c r="C285" t="s">
+        <v>784</v>
+      </c>
+      <c r="D285" t="s">
+        <v>785</v>
+      </c>
+      <c r="E285" t="s">
         <v>786</v>
-      </c>
-      <c r="D285" t="s">
-        <v>787</v>
-      </c>
-      <c r="E285" t="s">
-        <v>788</v>
       </c>
       <c r="F285" t="s">
         <v>14</v>
@@ -11107,13 +11107,13 @@
         <v>9</v>
       </c>
       <c r="C286" t="s">
+        <v>787</v>
+      </c>
+      <c r="D286" t="s">
+        <v>788</v>
+      </c>
+      <c r="E286" t="s">
         <v>789</v>
-      </c>
-      <c r="D286" t="s">
-        <v>790</v>
-      </c>
-      <c r="E286" t="s">
-        <v>791</v>
       </c>
       <c r="F286" t="s">
         <v>14</v>
@@ -11133,13 +11133,13 @@
         <v>9</v>
       </c>
       <c r="C287" t="s">
+        <v>790</v>
+      </c>
+      <c r="D287" t="s">
+        <v>791</v>
+      </c>
+      <c r="E287" t="s">
         <v>792</v>
-      </c>
-      <c r="D287" t="s">
-        <v>793</v>
-      </c>
-      <c r="E287" t="s">
-        <v>794</v>
       </c>
       <c r="F287" t="s">
         <v>14</v>
@@ -11159,13 +11159,13 @@
         <v>9</v>
       </c>
       <c r="C288" t="s">
+        <v>867</v>
+      </c>
+      <c r="D288" t="s">
+        <v>868</v>
+      </c>
+      <c r="E288" t="s">
         <v>869</v>
-      </c>
-      <c r="D288" t="s">
-        <v>870</v>
-      </c>
-      <c r="E288" t="s">
-        <v>871</v>
       </c>
       <c r="F288" t="s">
         <v>14</v>
@@ -11266,10 +11266,10 @@
         <v>441</v>
       </c>
       <c r="D292" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="E292" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="F292" t="s">
         <v>14</v>
@@ -11289,13 +11289,13 @@
         <v>9</v>
       </c>
       <c r="C293" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D293" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E293" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F293" t="s">
         <v>14</v>
@@ -11315,13 +11315,13 @@
         <v>9</v>
       </c>
       <c r="C294" t="s">
+        <v>507</v>
+      </c>
+      <c r="D294" t="s">
+        <v>508</v>
+      </c>
+      <c r="E294" t="s">
         <v>509</v>
-      </c>
-      <c r="D294" t="s">
-        <v>510</v>
-      </c>
-      <c r="E294" t="s">
-        <v>511</v>
       </c>
       <c r="F294" t="s">
         <v>14</v>
@@ -11341,13 +11341,13 @@
         <v>9</v>
       </c>
       <c r="C295" t="s">
+        <v>510</v>
+      </c>
+      <c r="D295" t="s">
+        <v>511</v>
+      </c>
+      <c r="E295" t="s">
         <v>512</v>
-      </c>
-      <c r="D295" t="s">
-        <v>513</v>
-      </c>
-      <c r="E295" t="s">
-        <v>514</v>
       </c>
       <c r="F295" t="s">
         <v>13</v>
@@ -11367,13 +11367,13 @@
         <v>9</v>
       </c>
       <c r="C296" t="s">
+        <v>513</v>
+      </c>
+      <c r="D296" t="s">
+        <v>514</v>
+      </c>
+      <c r="E296" t="s">
         <v>515</v>
-      </c>
-      <c r="D296" t="s">
-        <v>516</v>
-      </c>
-      <c r="E296" t="s">
-        <v>517</v>
       </c>
       <c r="F296" t="s">
         <v>13</v>
@@ -11393,13 +11393,13 @@
         <v>9</v>
       </c>
       <c r="C297" t="s">
+        <v>516</v>
+      </c>
+      <c r="D297" t="s">
+        <v>517</v>
+      </c>
+      <c r="E297" t="s">
         <v>518</v>
-      </c>
-      <c r="D297" t="s">
-        <v>519</v>
-      </c>
-      <c r="E297" t="s">
-        <v>520</v>
       </c>
       <c r="F297" t="s">
         <v>14</v>
@@ -11419,13 +11419,13 @@
         <v>9</v>
       </c>
       <c r="C298" t="s">
+        <v>519</v>
+      </c>
+      <c r="D298" t="s">
+        <v>520</v>
+      </c>
+      <c r="E298" t="s">
         <v>521</v>
-      </c>
-      <c r="D298" t="s">
-        <v>522</v>
-      </c>
-      <c r="E298" t="s">
-        <v>523</v>
       </c>
       <c r="F298" t="s">
         <v>13</v>
@@ -11445,13 +11445,13 @@
         <v>9</v>
       </c>
       <c r="C299" t="s">
+        <v>525</v>
+      </c>
+      <c r="D299" t="s">
+        <v>526</v>
+      </c>
+      <c r="E299" t="s">
         <v>527</v>
-      </c>
-      <c r="D299" t="s">
-        <v>528</v>
-      </c>
-      <c r="E299" t="s">
-        <v>529</v>
       </c>
       <c r="F299" t="s">
         <v>13</v>
@@ -11471,13 +11471,13 @@
         <v>9</v>
       </c>
       <c r="C300" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D300" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E300" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F300" t="s">
         <v>14</v>
@@ -11497,13 +11497,13 @@
         <v>9</v>
       </c>
       <c r="C301" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D301" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E301" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F301" t="s">
         <v>5</v>
@@ -11523,16 +11523,16 @@
         <v>9</v>
       </c>
       <c r="C302" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="D302" t="s">
+        <v>873</v>
+      </c>
+      <c r="E302" t="s">
         <v>875</v>
       </c>
-      <c r="E302" t="s">
-        <v>877</v>
-      </c>
       <c r="F302" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G302" t="s">
         <v>14</v>
@@ -11549,13 +11549,13 @@
         <v>9</v>
       </c>
       <c r="C303" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D303" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E303" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F303" t="s">
         <v>13</v>
@@ -11575,13 +11575,13 @@
         <v>9</v>
       </c>
       <c r="C304" t="s">
+        <v>599</v>
+      </c>
+      <c r="D304" t="s">
+        <v>600</v>
+      </c>
+      <c r="E304" t="s">
         <v>601</v>
-      </c>
-      <c r="D304" t="s">
-        <v>602</v>
-      </c>
-      <c r="E304" t="s">
-        <v>603</v>
       </c>
       <c r="F304" t="s">
         <v>13</v>
@@ -11601,13 +11601,13 @@
         <v>9</v>
       </c>
       <c r="C305" t="s">
+        <v>602</v>
+      </c>
+      <c r="D305" t="s">
+        <v>603</v>
+      </c>
+      <c r="E305" t="s">
         <v>604</v>
-      </c>
-      <c r="D305" t="s">
-        <v>605</v>
-      </c>
-      <c r="E305" t="s">
-        <v>606</v>
       </c>
       <c r="F305" t="s">
         <v>5</v>
@@ -11627,13 +11627,13 @@
         <v>9</v>
       </c>
       <c r="C306" t="s">
+        <v>615</v>
+      </c>
+      <c r="D306" t="s">
+        <v>616</v>
+      </c>
+      <c r="E306" t="s">
         <v>617</v>
-      </c>
-      <c r="D306" t="s">
-        <v>618</v>
-      </c>
-      <c r="E306" t="s">
-        <v>619</v>
       </c>
       <c r="F306" t="s">
         <v>14</v>
@@ -11653,13 +11653,13 @@
         <v>267</v>
       </c>
       <c r="C307" t="s">
+        <v>876</v>
+      </c>
+      <c r="D307" t="s">
+        <v>877</v>
+      </c>
+      <c r="E307" t="s">
         <v>878</v>
-      </c>
-      <c r="D307" t="s">
-        <v>879</v>
-      </c>
-      <c r="E307" t="s">
-        <v>880</v>
       </c>
       <c r="F307" t="s">
         <v>5</v>
@@ -11679,13 +11679,13 @@
         <v>267</v>
       </c>
       <c r="C308" t="s">
+        <v>879</v>
+      </c>
+      <c r="D308" t="s">
+        <v>880</v>
+      </c>
+      <c r="E308" t="s">
         <v>881</v>
-      </c>
-      <c r="D308" t="s">
-        <v>882</v>
-      </c>
-      <c r="E308" t="s">
-        <v>883</v>
       </c>
       <c r="F308" t="s">
         <v>5</v>
@@ -11708,10 +11708,10 @@
         <v>269</v>
       </c>
       <c r="D309" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E309" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="F309" t="s">
         <v>5</v>
@@ -11734,10 +11734,10 @@
         <v>272</v>
       </c>
       <c r="D310" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E310" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="F310" t="s">
         <v>5</v>
@@ -11760,10 +11760,10 @@
         <v>275</v>
       </c>
       <c r="D311" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E311" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="F311" t="s">
         <v>5</v>
@@ -11835,13 +11835,13 @@
         <v>267</v>
       </c>
       <c r="C314" t="s">
+        <v>609</v>
+      </c>
+      <c r="D314" t="s">
+        <v>610</v>
+      </c>
+      <c r="E314" t="s">
         <v>611</v>
-      </c>
-      <c r="D314" t="s">
-        <v>612</v>
-      </c>
-      <c r="E314" t="s">
-        <v>613</v>
       </c>
       <c r="F314" t="s">
         <v>13</v>
@@ -11861,13 +11861,13 @@
         <v>268</v>
       </c>
       <c r="C315" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D315" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E315" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="F315" t="s">
         <v>5</v>
@@ -11887,13 +11887,13 @@
         <v>268</v>
       </c>
       <c r="C316" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D316" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E316" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F316" t="s">
         <v>5</v>
@@ -11916,10 +11916,10 @@
         <v>269</v>
       </c>
       <c r="D317" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E317" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="F317" t="s">
         <v>5</v>
@@ -11942,10 +11942,10 @@
         <v>272</v>
       </c>
       <c r="D318" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E318" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="F318" t="s">
         <v>5</v>
@@ -11965,10 +11965,10 @@
         <v>268</v>
       </c>
       <c r="C319" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D319" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="E319" t="s">
         <v>343</v>
@@ -12017,13 +12017,13 @@
         <v>268</v>
       </c>
       <c r="C321" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D321" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E321" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F321" t="s">
         <v>14</v>
@@ -12043,13 +12043,13 @@
         <v>268</v>
       </c>
       <c r="C322" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D322" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E322" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F322" t="s">
         <v>14</v>
@@ -12101,7 +12101,7 @@
         <v>184</v>
       </c>
       <c r="E324" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F324" t="s">
         <v>5</v>
@@ -12121,13 +12121,13 @@
         <v>163</v>
       </c>
       <c r="C325" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="D325" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E325" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F325" t="s">
         <v>5</v>
@@ -12462,10 +12462,10 @@
         <v>441</v>
       </c>
       <c r="D338" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E338" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F338" t="s">
         <v>14</v>
@@ -12485,13 +12485,13 @@
         <v>163</v>
       </c>
       <c r="C339" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D339" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E339" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F339" t="s">
         <v>14</v>
@@ -12511,13 +12511,13 @@
         <v>163</v>
       </c>
       <c r="C340" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D340" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E340" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F340" t="s">
         <v>14</v>
@@ -12537,13 +12537,13 @@
         <v>163</v>
       </c>
       <c r="C341" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D341" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E341" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F341" t="s">
         <v>14</v>
@@ -12563,13 +12563,13 @@
         <v>163</v>
       </c>
       <c r="C342" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D342" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E342" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F342" t="s">
         <v>14</v>
@@ -12589,13 +12589,13 @@
         <v>163</v>
       </c>
       <c r="C343" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D343" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E343" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F343" t="s">
         <v>14</v>
@@ -12615,13 +12615,13 @@
         <v>163</v>
       </c>
       <c r="C344" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D344" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E344" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F344" t="s">
         <v>14</v>
@@ -12641,13 +12641,13 @@
         <v>163</v>
       </c>
       <c r="C345" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D345" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E345" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F345" t="s">
         <v>14</v>
@@ -12667,13 +12667,13 @@
         <v>163</v>
       </c>
       <c r="C346" t="s">
+        <v>573</v>
+      </c>
+      <c r="D346" t="s">
+        <v>574</v>
+      </c>
+      <c r="E346" t="s">
         <v>575</v>
-      </c>
-      <c r="D346" t="s">
-        <v>576</v>
-      </c>
-      <c r="E346" t="s">
-        <v>577</v>
       </c>
       <c r="F346" t="s">
         <v>14</v>
@@ -12693,13 +12693,13 @@
         <v>163</v>
       </c>
       <c r="C347" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D347" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E347" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F347" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Change name & lifeform for UNCHEN1 & 2 at PEFO to unknown chenopod (forb)
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/01b_edited-species8_location-dependent-final-fix.xlsx
+++ b/data/data-wrangling-intermediate/01b_edited-species8_location-dependent-final-fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:40009_{0BA8441D-1008-43DB-A010-9C50448DAA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D96AEDD-4F3D-47C9-9AB9-4B3D6D796CFB}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="13_ncr:40009_{0BA8441D-1008-43DB-A010-9C50448DAA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{826B5B0A-5D34-477C-8DFA-C6C07024CFA3}"/>
   <bookViews>
-    <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2515,18 +2515,12 @@
     <t>UCHEN1.PEFO</t>
   </si>
   <si>
-    <t>Unknown UCHEN1 (?), PEFO</t>
-  </si>
-  <si>
     <t>UCHEN2</t>
   </si>
   <si>
     <t>UCHEN2.PEFO</t>
   </si>
   <si>
-    <t>Unknown UCHEN2 (?), PEFO</t>
-  </si>
-  <si>
     <t>UNGR3.PEFO</t>
   </si>
   <si>
@@ -2741,6 +2735,12 @@
   </si>
   <si>
     <t>Unknown forb 5, AguaFria</t>
+  </si>
+  <si>
+    <t>Unknown chenopod 1, PEFO</t>
+  </si>
+  <si>
+    <t>Unknown chenopod 2, PEFO</t>
   </si>
 </sst>
 </file>
@@ -3680,8 +3680,8 @@
   <dimension ref="A1:H348"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4691,10 +4691,10 @@
         <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="D39" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E39" t="s">
         <v>223</v>
@@ -4876,10 +4876,10 @@
         <v>441</v>
       </c>
       <c r="D46" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="E46" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F46" t="s">
         <v>14</v>
@@ -4928,10 +4928,10 @@
         <v>465</v>
       </c>
       <c r="D48" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E48" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="F48" t="s">
         <v>14</v>
@@ -7479,7 +7479,7 @@
         <v>830</v>
       </c>
       <c r="E146" t="s">
-        <v>831</v>
+        <v>905</v>
       </c>
       <c r="F146" t="s">
         <v>14</v>
@@ -7488,7 +7488,7 @@
         <v>14</v>
       </c>
       <c r="H146" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
@@ -7499,13 +7499,13 @@
         <v>70</v>
       </c>
       <c r="C147" t="s">
+        <v>831</v>
+      </c>
+      <c r="D147" t="s">
         <v>832</v>
       </c>
-      <c r="D147" t="s">
-        <v>833</v>
-      </c>
       <c r="E147" t="s">
-        <v>834</v>
+        <v>906</v>
       </c>
       <c r="F147" t="s">
         <v>14</v>
@@ -7514,7 +7514,7 @@
         <v>14</v>
       </c>
       <c r="H147" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -7658,10 +7658,10 @@
         <v>573</v>
       </c>
       <c r="D153" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E153" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="F153" t="s">
         <v>5</v>
@@ -8747,13 +8747,13 @@
         <v>139</v>
       </c>
       <c r="C195" t="s">
+        <v>835</v>
+      </c>
+      <c r="D195" t="s">
+        <v>836</v>
+      </c>
+      <c r="E195" t="s">
         <v>837</v>
-      </c>
-      <c r="D195" t="s">
-        <v>838</v>
-      </c>
-      <c r="E195" t="s">
-        <v>839</v>
       </c>
       <c r="F195" t="s">
         <v>14</v>
@@ -9241,13 +9241,13 @@
         <v>145</v>
       </c>
       <c r="C214" t="s">
+        <v>838</v>
+      </c>
+      <c r="D214" t="s">
+        <v>839</v>
+      </c>
+      <c r="E214" t="s">
         <v>840</v>
-      </c>
-      <c r="D214" t="s">
-        <v>841</v>
-      </c>
-      <c r="E214" t="s">
-        <v>842</v>
       </c>
       <c r="F214" t="s">
         <v>14</v>
@@ -9267,13 +9267,13 @@
         <v>605</v>
       </c>
       <c r="C215" t="s">
+        <v>841</v>
+      </c>
+      <c r="D215" t="s">
+        <v>842</v>
+      </c>
+      <c r="E215" t="s">
         <v>843</v>
-      </c>
-      <c r="D215" t="s">
-        <v>844</v>
-      </c>
-      <c r="E215" t="s">
-        <v>845</v>
       </c>
       <c r="F215" t="s">
         <v>14</v>
@@ -10645,13 +10645,13 @@
         <v>9</v>
       </c>
       <c r="C268" t="s">
+        <v>844</v>
+      </c>
+      <c r="D268" t="s">
+        <v>845</v>
+      </c>
+      <c r="E268" t="s">
         <v>846</v>
-      </c>
-      <c r="D268" t="s">
-        <v>847</v>
-      </c>
-      <c r="E268" t="s">
-        <v>848</v>
       </c>
       <c r="F268" t="s">
         <v>5</v>
@@ -10671,13 +10671,13 @@
         <v>9</v>
       </c>
       <c r="C269" t="s">
+        <v>847</v>
+      </c>
+      <c r="D269" t="s">
+        <v>848</v>
+      </c>
+      <c r="E269" t="s">
         <v>849</v>
-      </c>
-      <c r="D269" t="s">
-        <v>850</v>
-      </c>
-      <c r="E269" t="s">
-        <v>851</v>
       </c>
       <c r="F269" t="s">
         <v>5</v>
@@ -10723,13 +10723,13 @@
         <v>9</v>
       </c>
       <c r="C271" t="s">
+        <v>850</v>
+      </c>
+      <c r="D271" t="s">
+        <v>851</v>
+      </c>
+      <c r="E271" t="s">
         <v>852</v>
-      </c>
-      <c r="D271" t="s">
-        <v>853</v>
-      </c>
-      <c r="E271" t="s">
-        <v>854</v>
       </c>
       <c r="F271" t="s">
         <v>5</v>
@@ -10749,13 +10749,13 @@
         <v>9</v>
       </c>
       <c r="C272" t="s">
+        <v>853</v>
+      </c>
+      <c r="D272" t="s">
+        <v>854</v>
+      </c>
+      <c r="E272" t="s">
         <v>855</v>
-      </c>
-      <c r="D272" t="s">
-        <v>856</v>
-      </c>
-      <c r="E272" t="s">
-        <v>857</v>
       </c>
       <c r="F272" t="s">
         <v>5</v>
@@ -10775,13 +10775,13 @@
         <v>9</v>
       </c>
       <c r="C273" t="s">
+        <v>856</v>
+      </c>
+      <c r="D273" t="s">
+        <v>857</v>
+      </c>
+      <c r="E273" t="s">
         <v>858</v>
-      </c>
-      <c r="D273" t="s">
-        <v>859</v>
-      </c>
-      <c r="E273" t="s">
-        <v>860</v>
       </c>
       <c r="F273" t="s">
         <v>5</v>
@@ -10801,13 +10801,13 @@
         <v>9</v>
       </c>
       <c r="C274" t="s">
+        <v>859</v>
+      </c>
+      <c r="D274" t="s">
+        <v>860</v>
+      </c>
+      <c r="E274" t="s">
         <v>861</v>
-      </c>
-      <c r="D274" t="s">
-        <v>862</v>
-      </c>
-      <c r="E274" t="s">
-        <v>863</v>
       </c>
       <c r="F274" t="s">
         <v>5</v>
@@ -10827,13 +10827,13 @@
         <v>9</v>
       </c>
       <c r="C275" t="s">
+        <v>862</v>
+      </c>
+      <c r="D275" t="s">
+        <v>863</v>
+      </c>
+      <c r="E275" t="s">
         <v>864</v>
-      </c>
-      <c r="D275" t="s">
-        <v>865</v>
-      </c>
-      <c r="E275" t="s">
-        <v>866</v>
       </c>
       <c r="F275" t="s">
         <v>5</v>
@@ -11191,13 +11191,13 @@
         <v>9</v>
       </c>
       <c r="C289" t="s">
+        <v>865</v>
+      </c>
+      <c r="D289" t="s">
+        <v>866</v>
+      </c>
+      <c r="E289" t="s">
         <v>867</v>
-      </c>
-      <c r="D289" t="s">
-        <v>868</v>
-      </c>
-      <c r="E289" t="s">
-        <v>869</v>
       </c>
       <c r="F289" t="s">
         <v>14</v>
@@ -11298,10 +11298,10 @@
         <v>441</v>
       </c>
       <c r="D293" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E293" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="F293" t="s">
         <v>14</v>
@@ -11555,13 +11555,13 @@
         <v>9</v>
       </c>
       <c r="C303" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="D303" t="s">
+        <v>871</v>
+      </c>
+      <c r="E303" t="s">
         <v>873</v>
-      </c>
-      <c r="E303" t="s">
-        <v>875</v>
       </c>
       <c r="F303" t="s">
         <v>726</v>
@@ -11587,7 +11587,7 @@
         <v>589</v>
       </c>
       <c r="E304" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="F304" t="s">
         <v>13</v>
@@ -11685,13 +11685,13 @@
         <v>267</v>
       </c>
       <c r="C308" t="s">
+        <v>874</v>
+      </c>
+      <c r="D308" t="s">
+        <v>875</v>
+      </c>
+      <c r="E308" t="s">
         <v>876</v>
-      </c>
-      <c r="D308" t="s">
-        <v>877</v>
-      </c>
-      <c r="E308" t="s">
-        <v>878</v>
       </c>
       <c r="F308" t="s">
         <v>5</v>
@@ -11711,13 +11711,13 @@
         <v>267</v>
       </c>
       <c r="C309" t="s">
+        <v>877</v>
+      </c>
+      <c r="D309" t="s">
+        <v>878</v>
+      </c>
+      <c r="E309" t="s">
         <v>879</v>
-      </c>
-      <c r="D309" t="s">
-        <v>880</v>
-      </c>
-      <c r="E309" t="s">
-        <v>881</v>
       </c>
       <c r="F309" t="s">
         <v>5</v>
@@ -11740,10 +11740,10 @@
         <v>269</v>
       </c>
       <c r="D310" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E310" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="F310" t="s">
         <v>5</v>
@@ -11766,10 +11766,10 @@
         <v>272</v>
       </c>
       <c r="D311" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E311" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="F311" t="s">
         <v>5</v>
@@ -11792,10 +11792,10 @@
         <v>275</v>
       </c>
       <c r="D312" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E312" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="F312" t="s">
         <v>5</v>
@@ -11893,13 +11893,13 @@
         <v>268</v>
       </c>
       <c r="C316" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="D316" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E316" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="F316" t="s">
         <v>5</v>
@@ -11919,13 +11919,13 @@
         <v>268</v>
       </c>
       <c r="C317" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D317" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E317" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="F317" t="s">
         <v>5</v>
@@ -11948,10 +11948,10 @@
         <v>269</v>
       </c>
       <c r="D318" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E318" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F318" t="s">
         <v>5</v>
@@ -11974,10 +11974,10 @@
         <v>272</v>
       </c>
       <c r="D319" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E319" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="F319" t="s">
         <v>5</v>
@@ -12078,10 +12078,10 @@
         <v>576</v>
       </c>
       <c r="D323" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E323" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="F323" t="s">
         <v>14</v>
@@ -12153,13 +12153,13 @@
         <v>163</v>
       </c>
       <c r="C326" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="D326" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E326" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="F326" t="s">
         <v>5</v>

</xml_diff>